<commit_message>
corrected sample.IDs in data files, added 12/5 CRM data, and made some TA plots
</commit_message>
<xml_diff>
--- a/Water_Chemistry/data/Apex/DatesToExclude.xlsx
+++ b/Water_Chemistry/data/Apex/DatesToExclude.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shelly/Documents/GitHub/P_generosa/Water_Chemistry/data/Apex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6AD5018-3BC4-0D40-954F-AA6438433461}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4BDD60-2D6F-F042-AECD-4B1A9AD3E314}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{5A0E5CD6-98EE-9740-A222-E00B489F4D86}"/>
+    <workbookView xWindow="3180" yWindow="460" windowWidth="27640" windowHeight="15540" xr2:uid="{5A0E5CD6-98EE-9740-A222-E00B489F4D86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,37 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t xml:space="preserve">cleaning </t>
+  </si>
+  <si>
+    <t>calibration</t>
+  </si>
+  <si>
+    <t>piloting</t>
+  </si>
+  <si>
+    <t>StartTime</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
+    <t>EndTime</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -60,8 +84,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,12 +402,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F63C978-1BD2-9F4C-AAE5-FAD3F55F0F7E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>43399</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>